<commit_message>
update replace virables to get just text
</commit_message>
<xml_diff>
--- a/dadada.xlsx
+++ b/dadada.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27726"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD4460E5-2F6B-4E0A-B98D-1F0CDAF2C735}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>name</t>
   </si>
@@ -39,29 +40,40 @@
     <t>file name</t>
   </si>
   <si>
-    <t>ATIF ALABBASI</t>
-  </si>
-  <si>
-    <t>dev@una-oic.org</t>
-  </si>
-  <si>
-    <t>Engineer</t>
-  </si>
-  <si>
-    <t>Telecommunications</t>
-  </si>
-  <si>
-    <t>file2.txt,file3.txt</t>
+    <t>عاطف العباسي</t>
+  </si>
+  <si>
+    <t>مهندس</t>
+  </si>
+  <si>
+    <t>crt_Part_1.pdf</t>
+  </si>
+  <si>
+    <t>Abbasi's-affection</t>
+  </si>
+  <si>
+    <t>الاستاذ</t>
+  </si>
+  <si>
+    <t>no5510425@gmail.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -84,13 +96,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -99,14 +114,17 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -144,7 +162,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -216,7 +234,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -389,11 +407,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:G2"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -425,32 +443,35 @@
       <c r="A2" t="s">
         <v>7</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" t="s">
         <v>8</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2">
+        <v>5</v>
+      </c>
+      <c r="F2" t="s">
         <v>9</v>
       </c>
-      <c r="D2" t="s">
+      <c r="G2" t="s">
         <v>10</v>
-      </c>
-      <c r="E2">
-        <v>9</v>
-      </c>
-      <c r="F2" t="s">
-        <v>11</v>
-      </c>
-      <c r="G2">
-        <v>13</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{B64F4706-9BF3-4EB8-A06D-2B9D4CE0D02E}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -462,7 +483,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>